<commit_message>
0.34.8:  Corrigido bug na função Spartacus.Utils.Excel.ReplaceMarkup
</commit_message>
<xml_diff>
--- a/Test/bin/Release/template_00001.xlsx
+++ b/Test/bin/Release/template_00001.xlsx
@@ -10,14 +10,14 @@
     <sheet name="ENTRADAS GERAL" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ENTRADAS GERAL'!$A$10:$AA$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ENTRADAS GERAL'!$A$11:$AC$11</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="66">
   <si>
     <t>Código Agente</t>
   </si>
@@ -100,9 +100,6 @@
     <t>*ST_AGN_ST_NOME</t>
   </si>
   <si>
-    <t>*ST_ENT_ST_SERIE</t>
-  </si>
-  <si>
     <t>*ST_ENT_ST_DI</t>
   </si>
   <si>
@@ -160,15 +157,9 @@
     <t>*IN_AGENTE</t>
   </si>
   <si>
-    <t>*ST_NOTA</t>
-  </si>
-  <si>
     <t>*ST_DATA</t>
   </si>
   <si>
-    <t>*ST_CFOP</t>
-  </si>
-  <si>
     <t>*ST_PRODUTO</t>
   </si>
   <si>
@@ -199,26 +190,62 @@
     <t>*ST_PAIS_ST_NOME</t>
   </si>
   <si>
-    <t>TIPO;CAMPO;POSICAO;OPCIONAL
-ST;titulo;A6;
-ST;filtro;A8;
-ST;ano;E2:J2;
-ST;empresa;E4:J4;
-IM;imagem;0:0;80
-TO;;M9;M11
-TO;;N9;N11
-TO;;O9;O11
-TO;;P9;P11
-TO;;Q9;Q11
-TO;;R9;R11
-TO;;S9;S11
-TO;;T9;T11
-TO;;U9;U11
-TO;;V9;V11
-TO;;W9;W11</t>
-  </si>
-  <si>
     <t>*subtotal</t>
+  </si>
+  <si>
+    <t>*IN_NOTA</t>
+  </si>
+  <si>
+    <t>*IN_ENT_ST_SERIE</t>
+  </si>
+  <si>
+    <t>*IN_CFOP</t>
+  </si>
+  <si>
+    <t>Prazo Pagamento</t>
+  </si>
+  <si>
+    <t>ICMS ST</t>
+  </si>
+  <si>
+    <t>*RE_ENT_IN_PRAZOPAGAMENTO</t>
+  </si>
+  <si>
+    <t>*RE_ENT_RE_ICMSST</t>
+  </si>
+  <si>
+    <t>TIPO|CAMPO|POSICAO|OPCIONAL
+ST|titulo|A6|
+ST|filtro|A8|
+ST|ano|E2:J2|
+ST|empresa|E4:J4|
+IM|imagem|0:0|80
+TO|SUM(#)|M9|M12
+TO|SUM(#)|N9|N12
+TO|SUM(#)|O9|O12
+TO|SUM(#)|P9|P12
+TO|SUM(#)|Q9|Q12
+TO|SUM(#)|R9|R12
+TO|SUM(#)|S9|S12
+TO|SUM(#)|T9|T12
+TO|SUM(#)|U9|U12
+TO|SUM(#)|V9|V12
+TO|SUM(#)|W9|W12
+TO|SUM(#)|X9|X12
+TO|SUM(#)|Y9|Y12
+TO|SUBTOTAL(9,#)|M10|M12
+TO|SUBTOTAL(9,#)|N10|N12
+TO|SUBTOTAL(9,#)|O10|O12
+TO|SUBTOTAL(9,#)|P10|P12
+TO|SUBTOTAL(9,#)|Q10|Q12
+TO|SUBTOTAL(9,#)|R10|R12
+TO|SUBTOTAL(9,#)|S10|S12
+TO|SUBTOTAL(9,#)|T10|T12
+TO|SUBTOTAL(9,#)|U10|U12
+TO|SUBTOTAL(9,#)|V10|V12
+TO|SUBTOTAL(9,#)|W10|W12
+TO|SUBTOTAL(9,#)|X10|X12
+TO|SUBTOTAL(9,#)|Y10|Y12</t>
   </si>
 </sst>
 </file>
@@ -287,7 +314,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -304,6 +331,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -599,11 +627,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB11"/>
+  <dimension ref="A1:AD12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M3" sqref="M3"/>
+      <pane ySplit="11" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -619,22 +647,25 @@
     <col min="20" max="20" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="22" max="24" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="10.5703125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="15" customHeight="1">
+    <row r="1" spans="1:30" ht="15" customHeight="1">
       <c r="A1" s="10" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="K1" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L1" s="1"/>
       <c r="M1" s="2"/>
       <c r="X1"/>
-    </row>
-    <row r="2" spans="1:28">
+      <c r="Y1"/>
+      <c r="Z1"/>
+    </row>
+    <row r="2" spans="1:30">
       <c r="E2" s="11" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F2" s="11"/>
       <c r="G2" s="11"/>
@@ -642,13 +673,15 @@
       <c r="I2" s="11"/>
       <c r="J2" s="11"/>
       <c r="K2" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L2" s="1"/>
       <c r="M2" s="2"/>
       <c r="X2"/>
-    </row>
-    <row r="3" spans="1:28">
+      <c r="Y2"/>
+      <c r="Z2"/>
+    </row>
+    <row r="3" spans="1:30">
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -656,15 +689,17 @@
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
       <c r="K3" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="2"/>
       <c r="X3"/>
-    </row>
-    <row r="4" spans="1:28">
+      <c r="Y3"/>
+      <c r="Z3"/>
+    </row>
+    <row r="4" spans="1:30">
       <c r="E4" s="11" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F4" s="11"/>
       <c r="G4" s="11"/>
@@ -672,28 +707,32 @@
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
       <c r="K4" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="2"/>
       <c r="X4"/>
-    </row>
-    <row r="5" spans="1:28">
+      <c r="Y4"/>
+      <c r="Z4"/>
+    </row>
+    <row r="5" spans="1:30">
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
       <c r="K5" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L5" s="1"/>
       <c r="M5" s="2"/>
       <c r="X5"/>
-    </row>
-    <row r="6" spans="1:28">
+      <c r="Y5"/>
+      <c r="Z5"/>
+    </row>
+    <row r="6" spans="1:30">
       <c r="A6" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
@@ -702,13 +741,15 @@
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
       <c r="K6" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L6" s="1"/>
       <c r="M6" s="2"/>
       <c r="X6"/>
-    </row>
-    <row r="7" spans="1:28">
+      <c r="Y6"/>
+      <c r="Z6"/>
+    </row>
+    <row r="7" spans="1:30">
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
@@ -716,275 +757,315 @@
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L7" s="1"/>
       <c r="M7" s="2"/>
       <c r="X7"/>
-    </row>
-    <row r="8" spans="1:28">
+      <c r="Y7"/>
+      <c r="Z7"/>
+    </row>
+    <row r="8" spans="1:30">
       <c r="A8" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
+        <v>54</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
       <c r="K8" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="L8" s="1"/>
+      <c r="M8" s="2"/>
+      <c r="X8"/>
+      <c r="Y8"/>
+      <c r="Z8"/>
+    </row>
+    <row r="9" spans="1:30">
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="K9" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="X9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z9" s="1"/>
+    </row>
+    <row r="10" spans="1:30">
+      <c r="K10" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="L10" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="U10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="V10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="W10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="X10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z10" s="1"/>
+    </row>
+    <row r="11" spans="1:30">
+      <c r="A11" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="N11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="O11" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="P11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q11" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="R11" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="S11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="T11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="U11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="V11" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="W11" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="X11" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y11" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z11" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC11" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD11" s="5"/>
+    </row>
+    <row r="12" spans="1:30">
+      <c r="A12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" t="s">
+        <v>59</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="H12" t="s">
+        <v>27</v>
+      </c>
+      <c r="I12" t="s">
+        <v>47</v>
+      </c>
+      <c r="J12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K12" t="s">
+        <v>29</v>
+      </c>
+      <c r="L12" t="s">
+        <v>30</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="R12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="S12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="T12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="U12" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="V12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="W12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="X12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y12" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC12" t="s">
         <v>44</v>
       </c>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="O8" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q8" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="R8" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="S8" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="T8" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="U8" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="V8" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="W8" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="X8" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="1:28">
-      <c r="K9" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="L9" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q9" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="R9" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="S9" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="T9" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="U9" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="V9" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="W9" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="X9" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="10" spans="1:28">
-      <c r="A10" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="K10" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="L10" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="M10" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="N10" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="O10" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="P10" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q10" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="R10" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="S10" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="T10" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="U10" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="V10" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="W10" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="X10" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="Y10" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="Z10" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="AA10" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="AB10" s="5"/>
-    </row>
-    <row r="11" spans="1:28">
-      <c r="A11" t="s">
-        <v>46</v>
-      </c>
-      <c r="B11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" t="s">
-        <v>59</v>
-      </c>
-      <c r="D11" t="s">
-        <v>47</v>
-      </c>
-      <c r="E11" t="s">
-        <v>27</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="G11" t="s">
-        <v>49</v>
-      </c>
-      <c r="H11" t="s">
-        <v>28</v>
-      </c>
-      <c r="I11" t="s">
-        <v>50</v>
-      </c>
-      <c r="J11" t="s">
-        <v>29</v>
-      </c>
-      <c r="K11" t="s">
-        <v>30</v>
-      </c>
-      <c r="L11" t="s">
-        <v>31</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="N11" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="O11" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="P11" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q11" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="R11" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="S11" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="T11" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="U11" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="V11" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="W11" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="X11" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="Y11" t="s">
-        <v>51</v>
-      </c>
-      <c r="Z11" t="s">
-        <v>52</v>
-      </c>
-      <c r="AA11" t="s">
-        <v>45</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A10:AA10">
+  <autoFilter ref="A11:AC11">
     <filterColumn colId="2"/>
+    <filterColumn colId="24"/>
+    <filterColumn colId="25"/>
   </autoFilter>
   <mergeCells count="2">
     <mergeCell ref="E2:J2"/>

</xml_diff>

<commit_message>
0.34.10: Corrigido bug na Spartacus.Reporting.Report.RenderGroup
</commit_message>
<xml_diff>
--- a/Test/bin/Release/template_00001.xlsx
+++ b/Test/bin/Release/template_00001.xlsx
@@ -7,10 +7,10 @@
     <workbookView xWindow="12345" yWindow="150" windowWidth="11280" windowHeight="9525"/>
   </bookViews>
   <sheets>
-    <sheet name="ENTRADAS GERAL" sheetId="1" r:id="rId1"/>
+    <sheet name="Entradas Geral" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ENTRADAS GERAL'!$A$11:$AC$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Entradas Geral'!$A$11:$AC$11</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
@@ -155,9 +155,6 @@
   </si>
   <si>
     <t>*IN_AGENTE</t>
-  </si>
-  <si>
-    <t>*ST_DATA</t>
   </si>
   <si>
     <t>*ST_PRODUTO</t>
@@ -246,6 +243,9 @@
 TO|SUBTOTAL(9,#)|W10|W12
 TO|SUBTOTAL(9,#)|X10|X12
 TO|SUBTOTAL(9,#)|Y10|Y12</t>
+  </si>
+  <si>
+    <t>*DT_DATA</t>
   </si>
 </sst>
 </file>
@@ -314,7 +314,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -328,10 +328,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -631,7 +632,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="11" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M7" sqref="M7"/>
+      <selection pane="bottomLeft" activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -652,7 +653,7 @@
   <sheetData>
     <row r="1" spans="1:30" ht="15" customHeight="1">
       <c r="A1" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K1" s="9" t="s">
         <v>43</v>
@@ -664,14 +665,14 @@
       <c r="Z1"/>
     </row>
     <row r="2" spans="1:30">
-      <c r="E2" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
+      <c r="E2" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
       <c r="K2" s="9" t="s">
         <v>43</v>
       </c>
@@ -698,14 +699,14 @@
       <c r="Z3"/>
     </row>
     <row r="4" spans="1:30">
-      <c r="E4" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
+      <c r="E4" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
       <c r="K4" s="9" t="s">
         <v>43</v>
       </c>
@@ -732,7 +733,7 @@
     </row>
     <row r="6" spans="1:30">
       <c r="A6" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
@@ -767,7 +768,7 @@
     </row>
     <row r="8" spans="1:30">
       <c r="A8" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
@@ -793,44 +794,44 @@
         <v>43</v>
       </c>
       <c r="L9" s="1"/>
-      <c r="M9" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q9" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="R9" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="S9" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="T9" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="U9" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="V9" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="W9" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="X9" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y9" s="1" t="s">
-        <v>50</v>
+      <c r="M9" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="N9" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="O9" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="P9" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q9" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="R9" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="S9" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="T9" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="U9" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="V9" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="W9" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="X9" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y9" s="13" t="s">
+        <v>49</v>
       </c>
       <c r="Z9" s="1"/>
     </row>
@@ -841,44 +842,44 @@
       <c r="L10" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="M10" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="O10" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q10" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="R10" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="S10" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="T10" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="U10" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="V10" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="W10" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="X10" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="Y10" s="1" t="s">
-        <v>57</v>
+      <c r="M10" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="N10" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="O10" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="P10" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q10" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="R10" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="S10" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="T10" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="U10" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="V10" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="W10" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="X10" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y10" s="13" t="s">
+        <v>56</v>
       </c>
       <c r="Z10" s="1"/>
     </row>
@@ -890,7 +891,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>2</v>
@@ -956,10 +957,10 @@
         <v>20</v>
       </c>
       <c r="Y11" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Z11" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AA11" s="5" t="s">
         <v>22</v>
@@ -980,25 +981,25 @@
         <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>56</v>
-      </c>
-      <c r="D12" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" t="s">
         <v>58</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="G12" s="11" t="s">
         <v>59</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>60</v>
       </c>
       <c r="H12" t="s">
         <v>27</v>
       </c>
       <c r="I12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J12" t="s">
         <v>28</v>
@@ -1009,53 +1010,53 @@
       <c r="L12" t="s">
         <v>30</v>
       </c>
-      <c r="M12" s="1" t="s">
+      <c r="M12" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="N12" s="2" t="s">
+      <c r="N12" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="O12" s="2" t="s">
+      <c r="O12" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="P12" s="2" t="s">
+      <c r="P12" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="Q12" s="2" t="s">
+      <c r="Q12" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="R12" s="2" t="s">
+      <c r="R12" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="S12" s="2" t="s">
+      <c r="S12" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="T12" s="2" t="s">
+      <c r="T12" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="U12" s="2" t="s">
+      <c r="U12" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="V12" s="2" t="s">
+      <c r="V12" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="W12" s="2" t="s">
+      <c r="W12" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="X12" s="2" t="s">
+      <c r="X12" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="Y12" s="2" t="s">
-        <v>64</v>
+      <c r="Y12" s="13" t="s">
+        <v>63</v>
       </c>
       <c r="Z12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AA12" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB12" t="s">
         <v>48</v>
-      </c>
-      <c r="AB12" t="s">
-        <v>49</v>
       </c>
       <c r="AC12" t="s">
         <v>44</v>

</xml_diff>

<commit_message>
0.34.11: Implementado pacote de relatórios Excel (um relatório em cada planilha, no mesmo arquivo XLSX).
</commit_message>
<xml_diff>
--- a/Test/bin/Release/template_00001.xlsx
+++ b/Test/bin/Release/template_00001.xlsx
@@ -209,6 +209,9 @@
   </si>
   <si>
     <t>*RE_ENT_RE_ICMSST</t>
+  </si>
+  <si>
+    <t>*DT_DATA</t>
   </si>
   <si>
     <t>TIPO|CAMPO|POSICAO|OPCIONAL
@@ -242,10 +245,9 @@
 TO|SUBTOTAL(9,#)|V10|V12
 TO|SUBTOTAL(9,#)|W10|W12
 TO|SUBTOTAL(9,#)|X10|X12
-TO|SUBTOTAL(9,#)|Y10|Y12</t>
-  </si>
-  <si>
-    <t>*DT_DATA</t>
+TO|SUBTOTAL(9,#)|Y10|Y12
+CF|#DBE5F1|A11:AD11|
+TA|A:AD|11|30</t>
   </si>
 </sst>
 </file>
@@ -329,10 +331,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -632,7 +634,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="11" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L9" sqref="L9"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -653,7 +655,7 @@
   <sheetData>
     <row r="1" spans="1:30" ht="15" customHeight="1">
       <c r="A1" s="10" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="K1" s="9" t="s">
         <v>43</v>
@@ -665,14 +667,14 @@
       <c r="Z1"/>
     </row>
     <row r="2" spans="1:30">
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
       <c r="K2" s="9" t="s">
         <v>43</v>
       </c>
@@ -699,14 +701,14 @@
       <c r="Z3"/>
     </row>
     <row r="4" spans="1:30">
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
       <c r="K4" s="9" t="s">
         <v>43</v>
       </c>
@@ -794,43 +796,43 @@
         <v>43</v>
       </c>
       <c r="L9" s="1"/>
-      <c r="M9" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="N9" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="O9" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="P9" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q9" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="R9" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="S9" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="T9" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="U9" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="V9" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="W9" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="X9" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="Y9" s="13" t="s">
+      <c r="M9" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="N9" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="O9" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="P9" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q9" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="R9" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="S9" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="T9" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="U9" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="V9" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="W9" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="X9" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y9" s="12" t="s">
         <v>49</v>
       </c>
       <c r="Z9" s="1"/>
@@ -842,43 +844,43 @@
       <c r="L10" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="M10" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="N10" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="O10" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="P10" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q10" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="R10" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="S10" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="T10" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="U10" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="V10" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="W10" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="X10" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="Y10" s="13" t="s">
+      <c r="M10" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="N10" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="O10" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="P10" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q10" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="R10" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="S10" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="T10" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="U10" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="V10" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="W10" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="X10" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y10" s="12" t="s">
         <v>56</v>
       </c>
       <c r="Z10" s="1"/>
@@ -990,7 +992,7 @@
         <v>58</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G12" s="11" t="s">
         <v>59</v>
@@ -1010,43 +1012,43 @@
       <c r="L12" t="s">
         <v>30</v>
       </c>
-      <c r="M12" s="13" t="s">
+      <c r="M12" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="N12" s="13" t="s">
+      <c r="N12" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="O12" s="13" t="s">
+      <c r="O12" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="P12" s="13" t="s">
+      <c r="P12" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="Q12" s="13" t="s">
+      <c r="Q12" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="R12" s="13" t="s">
+      <c r="R12" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="S12" s="13" t="s">
+      <c r="S12" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="T12" s="13" t="s">
+      <c r="T12" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="U12" s="13" t="s">
+      <c r="U12" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="V12" s="13" t="s">
+      <c r="V12" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="W12" s="13" t="s">
+      <c r="W12" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="X12" s="13" t="s">
+      <c r="X12" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="Y12" s="13" t="s">
+      <c r="Y12" s="12" t="s">
         <v>63</v>
       </c>
       <c r="Z12" t="s">

</xml_diff>

<commit_message>
0.34.12: Permitindo que o range de células do cabeçalho possa ser configurado na célula A1
</commit_message>
<xml_diff>
--- a/Test/bin/Release/template_00001.xlsx
+++ b/Test/bin/Release/template_00001.xlsx
@@ -215,6 +215,7 @@
   </si>
   <si>
     <t>TIPO|CAMPO|POSICAO|OPCIONAL
+CA||A1:AC12|
 ST|titulo|A6|
 ST|filtro|A8|
 ST|ano|E2:J2|
@@ -246,8 +247,8 @@
 TO|SUBTOTAL(9,#)|W10|W12
 TO|SUBTOTAL(9,#)|X10|X12
 TO|SUBTOTAL(9,#)|Y10|Y12
-CF|#DBE5F1|A11:AD11|
-TA|A:AD|11|30</t>
+CF|#DBE5F1|A11:AC11|
+TA|A:AC|11|29</t>
   </si>
 </sst>
 </file>
@@ -634,7 +635,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="11" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>